<commit_message>
Add Manual Testing project documentation
</commit_message>
<xml_diff>
--- a/Manual Testing/Test_Cases.xlsx
+++ b/Manual Testing/Test_Cases.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29518"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29602"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94A9890C-92F7-4C07-8A3E-0ACDE3F49DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B743BBDC-2E41-4AF7-B5B4-9ACA00F91BF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,25 +33,25 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="118">
   <si>
-    <t xml:space="preserve">ID </t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Precondition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Steps  </t>
+    <t>Test_case_ID</t>
+  </si>
+  <si>
+    <t>Test Scenario</t>
+  </si>
+  <si>
+    <t>Pre-Condition</t>
+  </si>
+  <si>
+    <t>Test Steps</t>
   </si>
   <si>
     <t>Test Data</t>
   </si>
   <si>
-    <t xml:space="preserve"> Expected Result</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Severity </t>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Severity</t>
   </si>
   <si>
     <t>Priority</t>
@@ -775,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -796,48 +796,48 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -868,7 +868,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1235,10 +1235,10 @@
       <c r="A18" t="s">
         <v>97</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>93</v>
       </c>
       <c r="D18" t="s">

</xml_diff>